<commit_message>
Logica per importare il file CN43N
</commit_message>
<xml_diff>
--- a/Solution/PptGeneratorGUI/DataSourceFolder/DataSource.xlsx
+++ b/Solution/PptGeneratorGUI/DataSourceFolder/DataSource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\PptGeneratorGUI\DataSourceFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4067ECE1-D3C1-4C20-95A0-570E7E33E4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EF5B40-BE92-42AF-A6CF-C6DA07123D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="924" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18071,7 +18071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5882B473-5D75-4EC5-97EA-2825D8D298DB}">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>